<commit_message>
correlation 5 and 6 - commons-lang
</commit_message>
<xml_diff>
--- a/correlation/correlation 5 and 6 - commons-lang .xlsx
+++ b/correlation/correlation 5 and 6 - commons-lang .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sl.No</t>
   </si>
@@ -32,22 +32,13 @@
   </si>
   <si>
     <t>Metrics 6</t>
-  </si>
-  <si>
-    <t>3.3.1</t>
-  </si>
-  <si>
-    <t>3.3.2</t>
-  </si>
-  <si>
-    <t>3.8.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -56,11 +47,16 @@
     <font>
       <b/>
     </font>
-    <font/>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,27 +86,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -355,15 +354,15 @@
       <c r="A4" s="3">
         <v>1.0</v>
       </c>
-      <c r="B4" s="3">
-        <v>3.3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2626.0</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D14" si="1">78+(0.01*C4)</f>
-        <v>104.26</v>
+      <c r="B4" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3046.0</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D9" si="1">78+(0.01*C4)</f>
+        <v>108.46</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -373,15 +372,15 @@
       <c r="A5" s="3">
         <v>2.0</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <v>163.0</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="B5" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>60259.0</v>
+      </c>
+      <c r="D5" s="5">
         <f t="shared" si="1"/>
-        <v>79.63</v>
+        <v>680.59</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -391,15 +390,15 @@
       <c r="A6" s="3">
         <v>3.0</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3">
-        <v>56.0</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2687.0</v>
+      </c>
+      <c r="D6" s="5">
         <f t="shared" si="1"/>
-        <v>78.56</v>
+        <v>104.87</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -412,12 +411,12 @@
       <c r="B7" s="3">
         <v>3.4</v>
       </c>
-      <c r="C7" s="3">
-        <v>4090.0</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="4">
+        <v>4368.0</v>
+      </c>
+      <c r="D7" s="5">
         <f t="shared" si="1"/>
-        <v>118.9</v>
+        <v>121.68</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -433,7 +432,7 @@
       <c r="C8" s="3">
         <v>10982.0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <f t="shared" si="1"/>
         <v>187.82</v>
       </c>
@@ -445,107 +444,61 @@
       <c r="A9" s="3">
         <v>6.0</v>
       </c>
-      <c r="B9" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7423.0</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="B9" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>36569.0</v>
+      </c>
+      <c r="D9" s="5">
         <f t="shared" si="1"/>
-        <v>152.23</v>
+        <v>443.69</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3027.0</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="1"/>
-        <v>108.27</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="B11" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1354.0</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="1"/>
-        <v>91.54</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="3">
-        <v>9.0</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="B13" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="C13" s="3">
-        <v>13821.0</v>
-      </c>
-      <c r="D13" s="4">
-        <f t="shared" si="1"/>
-        <v>216.21</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="B14" s="6">
-        <f>3.1</f>
-        <v>3.1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>16409.0</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="1"/>
-        <v>242.09</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>

</xml_diff>